<commit_message>
fix mac_ids in apis
</commit_message>
<xml_diff>
--- a/public/assets/product_stocks_bulk_format.xlsx
+++ b/public/assets/product_stocks_bulk_format.xlsx
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>EEF8EF65-AAAA-4410-B201-B6E1C4B9A486</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>major</t>
   </si>
@@ -45,6 +42,12 @@
   </si>
   <si>
     <t>product_uuid</t>
+  </si>
+  <si>
+    <t>KEEPR90628497 EEF8EF65-AAAA-4410-B201-B6E1C4B9A486</t>
+  </si>
+  <si>
+    <t>KEEPR90638498 EEF8EF65-AAAA-4410-B201-B6E1C4B9A486</t>
   </si>
 </sst>
 </file>
@@ -518,38 +521,38 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="topLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.75" customWidth="1"/>
-    <col min="2" max="2" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="31.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3">
         <v>9062</v>
@@ -558,15 +561,15 @@
         <v>8497</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3">
         <v>9063</v>
@@ -575,7 +578,7 @@
         <v>8498</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>

</xml_diff>